<commit_message>
Added Test results for the web application
</commit_message>
<xml_diff>
--- a/testing/webapp/Birthday_test_case.xlsx
+++ b/testing/webapp/Birthday_test_case.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="244">
   <si>
     <t>Test Plans</t>
   </si>
@@ -1174,40 +1174,100 @@
     </r>
   </si>
   <si>
-    <t>press submit with all fields empty</t>
-  </si>
-  <si>
-    <t>press submit with empty message filed</t>
-  </si>
-  <si>
-    <t>press submit with empty subject field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">press cancel </t>
-  </si>
-  <si>
-    <t>presss submit with all fields filled out and image added</t>
-  </si>
-  <si>
     <t>Birthdays</t>
   </si>
   <si>
-    <t>system should not allow it as subject is mandatory field and error message should appear stating 'subject empty'</t>
-  </si>
-  <si>
-    <t>system should allow it as message is not a mandatory field</t>
-  </si>
-  <si>
-    <t xml:space="preserve">system should return to home page </t>
-  </si>
-  <si>
-    <t>system should allow it and message should go to the employees</t>
-  </si>
-  <si>
-    <t>press browse to upload image</t>
-  </si>
-  <si>
-    <t>the system should allow the user to upload an image of a certain size</t>
+    <t>Submitting an Empty message. That is pressing send with all the fields empty.</t>
+  </si>
+  <si>
+    <t>Sending a subject only, which contains only special characters.</t>
+  </si>
+  <si>
+    <t>System should allow the message to be sent as the mandotary field has been filled.</t>
+  </si>
+  <si>
+    <t>Submitting a message without the subject.</t>
+  </si>
+  <si>
+    <t>System should deny the message from being sent since subject is a mandotary field.</t>
+  </si>
+  <si>
+    <t>Sending a message which contains an image which is more than 2MB large.</t>
+  </si>
+  <si>
+    <t>System should deny the message to be sent. It should return an error message indicating that subject field is missing.</t>
+  </si>
+  <si>
+    <t>System should deny the message to be sent. It should return an error message showing that the image is too large.</t>
+  </si>
+  <si>
+    <t>Sending a subject only.</t>
+  </si>
+  <si>
+    <t>Sending a message with an image size less than 2MB.</t>
+  </si>
+  <si>
+    <t>System should allow message to be sent. The image size meets requirements.</t>
+  </si>
+  <si>
+    <t>Uploading a non-image document(e.g a text file, word document, excel spreadsheet) on the image field.</t>
+  </si>
+  <si>
+    <t>The system should reject the file as it is not an image.</t>
+  </si>
+  <si>
+    <t>Sending the birthday message to a particular department.</t>
+  </si>
+  <si>
+    <t>The system should allow the message to be sent.</t>
+  </si>
+  <si>
+    <t>Sending the birthday message to all departments</t>
+  </si>
+  <si>
+    <t>Cancelling the message after filling all the fields</t>
+  </si>
+  <si>
+    <t>The system should clear all fields and the redirect to the home page.</t>
+  </si>
+  <si>
+    <t>Cancelling the message without any of the fields</t>
+  </si>
+  <si>
+    <t>System send message and redirects to home page.</t>
+  </si>
+  <si>
+    <t>Sending a message without target, i.e without chooing which group the message should be sent to</t>
+  </si>
+  <si>
+    <t>System should deny the message to be sent. There is no target to send it to.</t>
+  </si>
+  <si>
+    <t>System returns an error indicating that a recepient should be selected.</t>
+  </si>
+  <si>
+    <t>System denies the message from being sent</t>
+  </si>
+  <si>
+    <t>System should accept the image the send the message.</t>
+  </si>
+  <si>
+    <t>Attaching an image on the message.</t>
+  </si>
+  <si>
+    <t>The System rejects all images. It says that the extension is invalid</t>
+  </si>
+  <si>
+    <t>The option for all departments is not developed yet.</t>
+  </si>
+  <si>
+    <t>The system clears all the fields</t>
+  </si>
+  <si>
+    <t>The system should stay on the birthday page.</t>
+  </si>
+  <si>
+    <t>System remains on the birthday page.</t>
   </si>
 </sst>
 </file>
@@ -1238,7 +1298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1257,8 +1317,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1281,11 +1353,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1349,6 +1432,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2448,10 +2540,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,7 +2568,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2528,59 +2620,148 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C12" s="10"/>
-    </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
-        <v>213</v>
+        <v>219</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A13" s="10" t="s">
+        <v>221</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
         <v>214</v>
       </c>
       <c r="B14" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>237</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>234</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
         <v>218</v>
       </c>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>215</v>
-      </c>
-      <c r="B15" s="10" t="s">
+      <c r="B18" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="C15" s="10"/>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
+      <c r="C18" s="25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
         <v>222</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B19" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="C16" s="10"/>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>216</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="C17" s="10"/>
+      <c r="C19" s="25" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="C20" s="26" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="10" t="s">
+        <v>226</v>
+      </c>
+      <c r="B21" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="C22" s="25" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
+        <v>229</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
+        <v>231</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>242</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>243</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>